<commit_message>
mise à jour fichier excel
A ne pas prendre en compte
</commit_message>
<xml_diff>
--- a/uploads/Railway Facilities Construction Phase.xlsx
+++ b/uploads/Railway Facilities Construction Phase.xlsx
@@ -162,6 +162,41 @@
         </r>
       </text>
     </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Road Map of the Mbalam Mining Convention 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Railway Facilities mean the Mainline Railway, the Initial Spur Lines (which is the standard gauge heavy haul railway, located within the Railway Area, in the case of the territory of Cameroon connecting the junction of the Mainline Railway to the Mine Loading Area or the junction of the Mainline Railway to the Congo Border Terminal) and, and eventually as the case may be any Additional Spur Lines. 
+As per article 1 of the Convention defining Project Commissioning, the Contruction Phase with respect to the Railway Facilities begins from the Date of Entry into Force until Project Commissioning.
+The Railway Project Company is the entity in charge of the construction, procurement and exploitation of  the Railway Facilities, this in accordance with:
+1) the Railway Specifications detailed in the Railway Agreement which will describe the technical requirements of the Railway Faciliities based on the Railway Master Plan provided to the Railway Project Company by the State;
+2) the Railway Concession granted to the Railway Project Company, by the appropriate authority, the terms of which are equally set out in the Railway Agreement.
+It should be noted that the signing of the Railway Agreement Constitute a condition precedent to the Entry into Foce of the Convention (Cf condition precedents to fulfilled on or before May 29, 2014).  
+To this end, pursuant to the setting up of the Railway Project Company and the signing of the Railway Agreement, the contruction phase compliance with respect to Railway Facilities will consist in:
+- Obtaining the Railway Concession;
+- Requesting and obtaining the railway project lease;
+- Carrying out the design and construction of the Railway Facilities;
+- And proceeding with the Commissioning</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B7" authorId="1">
       <text>
         <r>
@@ -186,6 +221,41 @@
 In accordance with article 29.1(a) of the Convention, prior to commencing work on the Railway Area, the Railway Project Company shall prepare a waste management procedure and comply to it while performing the work.
 Where the work performed by a Contractor or Subcontractor, the waste management procedure is prepared by the said Contractor or Subcontractor and submitted to the Railway Project Company for approval. 
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Road Map of the Mbalam Mining Convention 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Railway Facilities mean the Mainline Railway, the Initial Spur Lines (which is the standard gauge heavy haul railway, located within the Railway Area, in the case of the territory of Cameroon connecting the junction of the Mainline Railway to the Mine Loading Area or the junction of the Mainline Railway to the Congo Border Terminal) and, and eventually as the case may be any Additional Spur Lines. 
+As per article 1 of the Convention defining Project Commissioning, the Contruction Phase with respect to the Railway Facilities begins from the Date of Entry into Force until Project Commissioning.
+The Railway Project Company is the entity in charge of the construction, procurement and exploitation of  the Railway Facilities, this in accordance with:
+1) the Railway Specifications detailed in the Railway Agreement which will describe the technical requirements of the Railway Faciliities based on the Railway Master Plan provided to the Railway Project Company by the State;
+2) the Railway Concession granted to the Railway Project Company, by the appropriate authority, the terms of which are equally set out in the Railway Agreement.
+It should be noted that the signing of the Railway Agreement Constitute a condition precedent to the Entry into Foce of the Convention (Cf condition precedents to fulfilled on or before May 29, 2014).  
+To this end, pursuant to the setting up of the Railway Project Company and the signing of the Railway Agreement, the contruction phase compliance with respect to Railway Facilities will consist in:
+- Obtaining the Railway Concession;
+- Requesting and obtaining the railway project lease;
+- Carrying out the design and construction of the Railway Facilities;
+- And proceeding with the Commissioning</t>
         </r>
       </text>
     </comment>
@@ -295,12 +365,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
-  <si>
-    <t>Monitoring Issue/ Category (1)</t>
-  </si>
-  <si>
-    <t>Required action or operation (what need to be done)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+  <si>
+    <t>Monitoring Items/ Category (1)</t>
+  </si>
+  <si>
+    <t>Required action or operation or process (what need to be done)</t>
   </si>
   <si>
     <t>Date for compliance (timeframe, deadline)</t>
@@ -330,7 +400,7 @@
     <t>Risk/sanction</t>
   </si>
   <si>
-    <t>Comments</t>
+    <t>Comment</t>
   </si>
   <si>
     <t>Cam Iron</t>
@@ -372,7 +442,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
@@ -432,20 +501,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -467,21 +529,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24994659260841701"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -490,158 +546,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,58 +564,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,186 +875,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:M9"/>
+  <dimension ref="A4:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:M9"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6" t="s">
+    <row r="5" spans="1:13">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="7"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="211.5" thickTop="1" thickBot="1">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:13" ht="210">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="12"/>
+      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="166.5" thickTop="1" thickBot="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:13" ht="165">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="9" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="9" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="16"/>
+      <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="286.5" thickTop="1" thickBot="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:13" ht="285">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9" t="s">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
+      <c r="M8" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A6:A9"/>
+  <mergeCells count="12">
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:J4"/>

</xml_diff>